<commit_message>
Results from July 23, 2020 05:10:20 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-23.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-23.xlsx
@@ -572,14 +572,10 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44034</v>
-      </c>
-      <c r="C3" t="n">
-        <v>33555</v>
-      </c>
-      <c r="D3" t="n">
-        <v>283</v>
-      </c>
+        <v>44035</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>464</v>
       </c>
@@ -896,22 +892,22 @@
         <v>44035</v>
       </c>
       <c r="C10" t="n">
-        <v>35246</v>
+        <v>36259</v>
       </c>
       <c r="D10" t="n">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="E10" t="n">
-        <v>7521</v>
+        <v>7710</v>
       </c>
       <c r="F10" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G10" t="n">
-        <v>24.57</v>
+        <v>24.54</v>
       </c>
       <c r="H10" t="n">
-        <v>26.53</v>
+        <v>26.36</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -920,10 +916,10 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>30608</v>
+        <v>31419</v>
       </c>
       <c r="L10" t="n">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="M10" t="n">
         <v>460970</v>
@@ -944,25 +940,25 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44034</v>
+        <v>44035</v>
       </c>
       <c r="C11" t="n">
-        <v>25107</v>
+        <v>25608</v>
       </c>
       <c r="D11" t="n">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="E11" t="n">
-        <v>918</v>
+        <v>942</v>
       </c>
       <c r="F11" t="n">
         <v>19</v>
       </c>
       <c r="G11" t="n">
-        <v>4.67</v>
+        <v>4.7</v>
       </c>
       <c r="H11" t="n">
-        <v>3.85</v>
+        <v>3.81</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -971,10 +967,10 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>19655</v>
+        <v>20033</v>
       </c>
       <c r="L11" t="n">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="M11" t="n">
         <v>166412</v>
@@ -1042,16 +1038,16 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44034</v>
+        <v>44035</v>
       </c>
       <c r="C13" t="n">
-        <v>17828</v>
+        <v>18163</v>
       </c>
       <c r="D13" t="n">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="E13" t="n">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
@@ -1226,25 +1222,25 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C17" t="n">
-        <v>164870</v>
+        <v>166848</v>
       </c>
       <c r="D17" t="n">
-        <v>4213</v>
+        <v>4262</v>
       </c>
       <c r="E17" t="n">
-        <v>4391</v>
+        <v>4451</v>
       </c>
       <c r="F17" t="n">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="G17" t="n">
         <v>4.64</v>
       </c>
       <c r="H17" t="n">
-        <v>10.67</v>
+        <v>10.66</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1253,10 +1249,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>94674</v>
+        <v>95952</v>
       </c>
       <c r="L17" t="n">
-        <v>3927</v>
+        <v>3976</v>
       </c>
       <c r="M17" t="n">
         <v>823987</v>
@@ -1662,25 +1658,25 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44034</v>
+        <v>44035</v>
       </c>
       <c r="C27" t="n">
-        <v>41698</v>
+        <v>42314</v>
       </c>
       <c r="D27" t="n">
-        <v>1771</v>
+        <v>1786</v>
       </c>
       <c r="E27" t="n">
-        <v>2027</v>
+        <v>2048</v>
       </c>
       <c r="F27" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G27" t="n">
-        <v>6.17</v>
+        <v>6.16</v>
       </c>
       <c r="H27" t="n">
-        <v>6.89</v>
+        <v>6.9</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
@@ -1689,10 +1685,10 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>32858</v>
+        <v>33225</v>
       </c>
       <c r="L27" t="n">
-        <v>1713</v>
+        <v>1725</v>
       </c>
       <c r="M27" t="n">
         <v>227938</v>
@@ -1713,25 +1709,25 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44034</v>
+        <v>44035</v>
       </c>
       <c r="C28" t="n">
-        <v>23486</v>
+        <v>23818</v>
       </c>
       <c r="D28" t="n">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="E28" t="n">
-        <v>1390</v>
+        <v>1414</v>
       </c>
       <c r="F28" t="n">
         <v>23</v>
       </c>
       <c r="G28" t="n">
-        <v>7.65</v>
+        <v>7.69</v>
       </c>
       <c r="H28" t="n">
-        <v>7.74</v>
+        <v>7.72</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
@@ -1740,10 +1736,10 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>18180</v>
+        <v>18381</v>
       </c>
       <c r="L28" t="n">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M28" t="n">
         <v>90860</v>
@@ -2109,25 +2105,25 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44034</v>
+        <v>44035</v>
       </c>
       <c r="C36" t="n">
-        <v>49247</v>
+        <v>50009</v>
       </c>
       <c r="D36" t="n">
-        <v>1468</v>
+        <v>1482</v>
       </c>
       <c r="E36" t="n">
-        <v>1743</v>
+        <v>1766</v>
       </c>
       <c r="F36" t="n">
         <v>49</v>
       </c>
       <c r="G36" t="n">
-        <v>5.44</v>
+        <v>5.46</v>
       </c>
       <c r="H36" t="n">
-        <v>3.47</v>
+        <v>3.39</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -2136,10 +2132,10 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>32066</v>
+        <v>32323</v>
       </c>
       <c r="L36" t="n">
-        <v>1413</v>
+        <v>1446</v>
       </c>
       <c r="M36" t="n">
         <v>269854</v>
@@ -2262,7 +2258,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... HTTPError('504 Server Error: Gateway Time-out for url: https://myhealthycommunity.dhss.delaware.gov/locations/state/')</t>
+          <t>An error occurred. ... AttributeError("'numpy.float64' object has no attribute 'split'")</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 23, 2020 05:33:54 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-23.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-23.xlsx
@@ -574,8 +574,12 @@
       <c r="B3" s="2" t="n">
         <v>44035</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>34633</v>
+      </c>
+      <c r="D3" t="n">
+        <v>298</v>
+      </c>
       <c r="E3" t="n">
         <v>464</v>
       </c>

</xml_diff>

<commit_message>
Results from 2020-07-23 9:00 PM America/Los_Angeles run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-23.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-23.xlsx
@@ -73,74 +73,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -521,29 +453,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C2" t="n">
-        <v>30343</v>
+        <v>166925</v>
       </c>
       <c r="D2" t="n">
-        <v>774</v>
+        <v>7367</v>
       </c>
       <c r="E2" t="n">
-        <v>3644</v>
+        <v>27933</v>
       </c>
       <c r="F2" t="n">
-        <v>96</v>
+        <v>2027</v>
       </c>
       <c r="G2" t="n">
-        <v>0.12</v>
+        <v>16.73</v>
       </c>
       <c r="H2" t="n">
-        <v>0.12</v>
+        <v>27.51</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -554,10 +486,10 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>3365783</v>
+        <v>1824125</v>
       </c>
       <c r="N2" t="n">
-        <v>12.07</v>
+        <v>14.23</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -568,47 +500,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Texas -- Bexar County</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44035</v>
+        <v>44034</v>
       </c>
       <c r="C3" t="n">
-        <v>34633</v>
+        <v>101650</v>
       </c>
       <c r="D3" t="n">
-        <v>298</v>
+        <v>3574</v>
       </c>
       <c r="E3" t="n">
-        <v>464</v>
+        <v>36693</v>
       </c>
       <c r="F3" t="n">
-        <v>17</v>
+        <v>1803</v>
       </c>
       <c r="G3" t="n">
-        <v>6.81</v>
+        <v>45.36</v>
       </c>
       <c r="H3" t="n">
-        <v>15.32</v>
+        <v>51.05</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="J3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>6812</v>
+        <v>80885</v>
       </c>
       <c r="L3" t="n">
-        <v>111</v>
+        <v>3532</v>
       </c>
       <c r="M3" t="n">
-        <v>146703</v>
+        <v>1502916</v>
       </c>
       <c r="N3" t="n">
-        <v>7.62</v>
+        <v>32.23</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -619,51 +551,47 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>New York -- New York</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
         <v>44035</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>219489</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18839</t>
-        </is>
+      <c r="C4" t="n">
+        <v>50009</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1482</v>
       </c>
       <c r="E4" t="n">
-        <v>33830</v>
+        <v>1766</v>
       </c>
       <c r="F4" t="n">
-        <v>5244</v>
+        <v>49</v>
       </c>
       <c r="G4" t="n">
-        <v>30.06</v>
+        <v>5.46</v>
       </c>
       <c r="H4" t="n">
-        <v>30.42</v>
+        <v>3.39</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>112527</v>
+        <v>32323</v>
       </c>
       <c r="L4" t="n">
-        <v>17236</v>
+        <v>1446</v>
       </c>
       <c r="M4" t="n">
-        <v>2049418</v>
+        <v>269854</v>
       </c>
       <c r="N4" t="n">
-        <v>24.27</v>
+        <v>3.7</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -674,47 +602,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rhode Island</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44015</v>
+        <v>44035</v>
       </c>
       <c r="C5" t="n">
-        <v>16491</v>
+        <v>106893</v>
       </c>
       <c r="D5" t="n">
-        <v>960</v>
+        <v>1726</v>
       </c>
       <c r="E5" t="n">
-        <v>1592</v>
+        <v>17818</v>
       </c>
       <c r="F5" t="n">
-        <v>48</v>
+        <v>542</v>
       </c>
       <c r="G5" t="n">
-        <v>12.29</v>
+        <v>24.01</v>
       </c>
       <c r="H5" t="n">
-        <v>6.14</v>
+        <v>32.55</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>12950</v>
+        <v>74222</v>
       </c>
       <c r="L5" t="n">
-        <v>782</v>
+        <v>1665</v>
       </c>
       <c r="M5" t="n">
-        <v>69254</v>
+        <v>2179622</v>
       </c>
       <c r="N5" t="n">
-        <v>6.55</v>
+        <v>21.46</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -725,72 +653,102 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>California - San Francisco</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+          <t>New York -- New York</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>44035</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>219489</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>18839</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>33830</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5244</v>
+      </c>
+      <c r="G6" t="n">
+        <v>30.06</v>
+      </c>
+      <c r="H6" t="n">
+        <v>30.42</v>
+      </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>112527</v>
+      </c>
+      <c r="L6" t="n">
+        <v>17236</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2049418</v>
+      </c>
+      <c r="N6" t="n">
+        <v>24.27</v>
+      </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 85', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C7" t="n">
-        <v>86987</v>
+        <v>45899</v>
       </c>
       <c r="D7" t="n">
-        <v>925</v>
+        <v>878</v>
       </c>
       <c r="E7" t="n">
-        <v>17171</v>
+        <v>7222</v>
       </c>
       <c r="F7" t="n">
-        <v>325</v>
+        <v>198</v>
       </c>
       <c r="G7" t="n">
-        <v>19.74</v>
+        <v>17.43</v>
       </c>
       <c r="H7" t="n">
-        <v>35.14</v>
+        <v>22.97</v>
       </c>
       <c r="I7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>41432</v>
+      </c>
+      <c r="L7" t="n">
+        <v>862</v>
+      </c>
       <c r="M7" t="n">
-        <v>1117489</v>
+        <v>368744</v>
       </c>
       <c r="N7" t="n">
-        <v>16.8</v>
+        <v>6.38</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -801,51 +759,47 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Wisconsin -- Milwaukee</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
         <v>44035</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>36099</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>267</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>902</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="C8" t="n">
+        <v>17162</v>
+      </c>
+      <c r="D8" t="n">
+        <v>374</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4842</v>
+      </c>
+      <c r="F8" t="n">
+        <v>147</v>
       </c>
       <c r="G8" t="n">
-        <v>2.5</v>
+        <v>30.44</v>
       </c>
       <c r="H8" t="n">
-        <v>1.87</v>
+        <v>39.3</v>
       </c>
       <c r="I8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>15909</v>
+      </c>
+      <c r="L8" t="n">
+        <v>374</v>
+      </c>
       <c r="M8" t="n">
-        <v>35862</v>
+        <v>252321</v>
       </c>
       <c r="N8" t="n">
-        <v>1.18</v>
+        <v>26.44</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -856,80 +810,94 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kentucky</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+          <t>Rhode Island</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>44015</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16491</v>
+      </c>
+      <c r="D9" t="n">
+        <v>960</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1592</v>
+      </c>
+      <c r="F9" t="n">
+        <v>48</v>
+      </c>
+      <c r="G9" t="n">
+        <v>12.29</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6.14</v>
+      </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>12950</v>
+      </c>
+      <c r="L9" t="n">
+        <v>782</v>
+      </c>
       <c r="M9" t="n">
-        <v>354112</v>
+        <v>69254</v>
       </c>
       <c r="N9" t="n">
-        <v>7.98</v>
+        <v>6.55</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>An error occurred. ... UnboundLocalError("local variable 'aa_deaths_pct' referenced before assignment")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C10" t="n">
-        <v>36259</v>
+        <v>86987</v>
       </c>
       <c r="D10" t="n">
-        <v>386</v>
+        <v>925</v>
       </c>
       <c r="E10" t="n">
-        <v>7710</v>
+        <v>17171</v>
       </c>
       <c r="F10" t="n">
-        <v>102</v>
+        <v>325</v>
       </c>
       <c r="G10" t="n">
-        <v>24.54</v>
+        <v>19.74</v>
       </c>
       <c r="H10" t="n">
-        <v>26.36</v>
+        <v>35.14</v>
       </c>
       <c r="I10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
       </c>
-      <c r="K10" t="n">
-        <v>31419</v>
-      </c>
-      <c r="L10" t="n">
-        <v>387</v>
-      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
-        <v>460970</v>
+        <v>1117489</v>
       </c>
       <c r="N10" t="n">
-        <v>15.41</v>
+        <v>16.8</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -940,47 +908,41 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>California - San Diego</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C11" t="n">
-        <v>25608</v>
+        <v>3736</v>
       </c>
       <c r="D11" t="n">
-        <v>512</v>
+        <v>118</v>
       </c>
       <c r="E11" t="n">
-        <v>942</v>
-      </c>
-      <c r="F11" t="n">
-        <v>19</v>
-      </c>
+        <v>850</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="H11" t="n">
-        <v>3.81</v>
-      </c>
+        <v>25.3</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="b">
         <v>0</v>
       </c>
       <c r="J11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>20033</v>
-      </c>
-      <c r="L11" t="n">
-        <v>499</v>
-      </c>
+        <v>3360</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>166412</v>
+        <v>17881</v>
       </c>
       <c r="N11" t="n">
-        <v>5.04</v>
+        <v>1.34</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -991,43 +953,47 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44033</v>
+        <v>44035</v>
       </c>
       <c r="C12" t="n">
-        <v>79371</v>
+        <v>80836</v>
       </c>
       <c r="D12" t="n">
-        <v>2048</v>
+        <v>3281</v>
       </c>
       <c r="E12" t="n">
-        <v>12922</v>
+        <v>23905</v>
       </c>
       <c r="F12" t="n">
-        <v>483</v>
+        <v>1340</v>
       </c>
       <c r="G12" t="n">
-        <v>16.28</v>
+        <v>35.6</v>
       </c>
       <c r="H12" t="n">
-        <v>23.58</v>
+        <v>40.95</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>67144</v>
+      </c>
+      <c r="L12" t="n">
+        <v>3272</v>
+      </c>
       <c r="M12" t="n">
-        <v>1613285</v>
+        <v>1788090</v>
       </c>
       <c r="N12" t="n">
-        <v>19.17</v>
+        <v>29.78</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1038,39 +1004,47 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C13" t="n">
-        <v>18163</v>
+        <v>72696</v>
       </c>
       <c r="D13" t="n">
-        <v>596</v>
+        <v>1357</v>
       </c>
       <c r="E13" t="n">
-        <v>328</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
+        <v>21260</v>
+      </c>
+      <c r="F13" t="n">
+        <v>575</v>
+      </c>
       <c r="G13" t="n">
-        <v>1.81</v>
-      </c>
-      <c r="H13" t="inlineStr"/>
+        <v>43.53</v>
+      </c>
+      <c r="H13" t="n">
+        <v>44.44</v>
+      </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
       </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>48842</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1294</v>
+      </c>
       <c r="M13" t="n">
-        <v>43006</v>
+        <v>1293186</v>
       </c>
       <c r="N13" t="n">
-        <v>2.06</v>
+        <v>26.58</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1081,26 +1055,30 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Florida -- Miami-Dade County</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C14" t="n">
-        <v>95068</v>
+        <v>36259</v>
       </c>
       <c r="D14" t="n">
-        <v>1354</v>
+        <v>386</v>
       </c>
       <c r="E14" t="n">
-        <v>9136</v>
-      </c>
-      <c r="F14" t="inlineStr"/>
+        <v>7710</v>
+      </c>
+      <c r="F14" t="n">
+        <v>102</v>
+      </c>
       <c r="G14" t="n">
-        <v>19.38</v>
-      </c>
-      <c r="H14" t="inlineStr"/>
+        <v>24.54</v>
+      </c>
+      <c r="H14" t="n">
+        <v>26.36</v>
+      </c>
       <c r="I14" t="b">
         <v>0</v>
       </c>
@@ -1108,14 +1086,16 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>47152</v>
-      </c>
-      <c r="L14" t="inlineStr"/>
+        <v>31419</v>
+      </c>
+      <c r="L14" t="n">
+        <v>387</v>
+      </c>
       <c r="M14" t="n">
-        <v>481976</v>
+        <v>460970</v>
       </c>
       <c r="N14" t="n">
-        <v>17.75</v>
+        <v>15.41</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1126,41 +1106,43 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Florida -- Orange County</t>
+          <t>Connecticut</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44035</v>
+        <v>44034</v>
       </c>
       <c r="C15" t="n">
-        <v>25254</v>
+        <v>46213</v>
       </c>
       <c r="D15" t="n">
-        <v>156</v>
+        <v>3530</v>
       </c>
       <c r="E15" t="n">
-        <v>3205</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
+        <v>6382</v>
+      </c>
+      <c r="F15" t="n">
+        <v>653</v>
+      </c>
       <c r="G15" t="n">
-        <v>25.12</v>
-      </c>
-      <c r="H15" t="inlineStr"/>
+        <v>13.81</v>
+      </c>
+      <c r="H15" t="n">
+        <v>18.5</v>
+      </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" t="n">
-        <v>12758</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>277193</v>
+        <v>378262</v>
       </c>
       <c r="N15" t="n">
-        <v>20.98</v>
+        <v>10.56</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1171,47 +1153,43 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C16" t="n">
-        <v>72696</v>
+        <v>75868</v>
       </c>
       <c r="D16" t="n">
-        <v>1357</v>
+        <v>6065</v>
       </c>
       <c r="E16" t="n">
-        <v>21260</v>
+        <v>21684</v>
       </c>
       <c r="F16" t="n">
-        <v>575</v>
+        <v>2418</v>
       </c>
       <c r="G16" t="n">
-        <v>43.53</v>
+        <v>28.58</v>
       </c>
       <c r="H16" t="n">
-        <v>44.44</v>
+        <v>39.87</v>
       </c>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
       </c>
-      <c r="K16" t="n">
-        <v>48842</v>
-      </c>
-      <c r="L16" t="n">
-        <v>1294</v>
-      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
-        <v>1293186</v>
+        <v>1375424</v>
       </c>
       <c r="N16" t="n">
-        <v>26.58</v>
+        <v>13.81</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1222,47 +1200,39 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>California - Los Angeles</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44034</v>
+        <v>44035</v>
       </c>
       <c r="C17" t="n">
-        <v>166848</v>
+        <v>2910</v>
       </c>
       <c r="D17" t="n">
-        <v>4262</v>
+        <v>43</v>
       </c>
       <c r="E17" t="n">
-        <v>4451</v>
-      </c>
-      <c r="F17" t="n">
-        <v>424</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
-        <v>4.64</v>
-      </c>
-      <c r="H17" t="n">
-        <v>10.66</v>
-      </c>
+        <v>0.58</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" t="n">
-        <v>95952</v>
-      </c>
-      <c r="L17" t="n">
-        <v>3976</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
-        <v>823987</v>
+        <v>4630</v>
       </c>
       <c r="N17" t="n">
-        <v>8.16</v>
+        <v>0.44</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1273,76 +1243,98 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Maryland</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+          <t>Kansas</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>44034</v>
+      </c>
+      <c r="C18" t="n">
+        <v>24104</v>
+      </c>
+      <c r="D18" t="n">
+        <v>308</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1780</v>
+      </c>
+      <c r="F18" t="n">
+        <v>64</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9.029999999999999</v>
+      </c>
+      <c r="H18" t="n">
+        <v>21.33</v>
+      </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>19703</v>
+      </c>
+      <c r="L18" t="n">
+        <v>300</v>
+      </c>
       <c r="M18" t="n">
-        <v>1788090</v>
+        <v>169801</v>
       </c>
       <c r="N18" t="n">
-        <v>29.78</v>
+        <v>5.84</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 85', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mississippi</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44034</v>
+        <v>44035</v>
       </c>
       <c r="C19" t="n">
-        <v>48053</v>
+        <v>2192</v>
       </c>
       <c r="D19" t="n">
-        <v>1436</v>
+        <v>19</v>
       </c>
       <c r="E19" t="n">
-        <v>21106</v>
+        <v>52</v>
       </c>
       <c r="F19" t="n">
-        <v>722</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>43.92</v>
+        <v>3.82</v>
       </c>
       <c r="H19" t="n">
-        <v>50.28</v>
+        <v>0</v>
       </c>
       <c r="I19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="b">
         <v>1</v>
       </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
+      <c r="K19" t="n">
+        <v>1361</v>
+      </c>
+      <c r="L19" t="n">
+        <v>19</v>
+      </c>
       <c r="M19" t="n">
-        <v>1125834</v>
+        <v>24129</v>
       </c>
       <c r="N19" t="n">
-        <v>37.67</v>
+        <v>3.27</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1353,18 +1345,32 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Arizona</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+          <t>Massachusetts</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>44035</v>
+      </c>
+      <c r="C20" t="n">
+        <v>114647</v>
+      </c>
+      <c r="D20" t="n">
+        <v>8484</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10759</v>
+      </c>
+      <c r="F20" t="n">
+        <v>696</v>
+      </c>
+      <c r="G20" t="n">
+        <v>9.380000000000001</v>
+      </c>
+      <c r="H20" t="n">
+        <v>8.199999999999999</v>
+      </c>
       <c r="I20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="b">
         <v>0</v>
@@ -1372,44 +1378,40 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>305259</v>
+        <v>510558</v>
       </c>
       <c r="N20" t="n">
-        <v>4.39</v>
+        <v>7.48</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 85', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Pennsylvania</t>
+          <t>Florida -- Miami-Dade County</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C21" t="n">
-        <v>101408</v>
+        <v>95068</v>
       </c>
       <c r="D21" t="n">
-        <v>7079</v>
+        <v>1354</v>
       </c>
       <c r="E21" t="n">
-        <v>14220</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1484</v>
-      </c>
+        <v>9136</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>30.01</v>
-      </c>
-      <c r="H21" t="n">
-        <v>21.22</v>
-      </c>
+        <v>19.38</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="b">
         <v>0</v>
       </c>
@@ -1417,16 +1419,14 @@
         <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>47386</v>
-      </c>
-      <c r="L21" t="n">
-        <v>6992</v>
-      </c>
+        <v>47152</v>
+      </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>1423319</v>
+        <v>481976</v>
       </c>
       <c r="N21" t="n">
-        <v>11.13</v>
+        <v>17.75</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1437,43 +1437,41 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Florida -- Orange County</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C22" t="n">
-        <v>385091</v>
+        <v>25254</v>
       </c>
       <c r="D22" t="n">
-        <v>5518</v>
+        <v>156</v>
       </c>
       <c r="E22" t="n">
-        <v>46054</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1055</v>
-      </c>
+        <v>3205</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
-        <v>11.96</v>
-      </c>
-      <c r="H22" t="n">
-        <v>19.12</v>
-      </c>
+        <v>25.12</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>12758</v>
+      </c>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
-        <v>3316376</v>
+        <v>277193</v>
       </c>
       <c r="N22" t="n">
-        <v>16.1</v>
+        <v>20.98</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -1484,26 +1482,30 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C23" t="n">
-        <v>2910</v>
+        <v>40770</v>
       </c>
       <c r="D23" t="n">
-        <v>43</v>
+        <v>820</v>
       </c>
       <c r="E23" t="n">
-        <v>17</v>
-      </c>
-      <c r="F23" t="inlineStr"/>
+        <v>3317</v>
+      </c>
+      <c r="F23" t="n">
+        <v>38</v>
+      </c>
       <c r="G23" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="H23" t="inlineStr"/>
+        <v>8.140000000000001</v>
+      </c>
+      <c r="H23" t="n">
+        <v>4.63</v>
+      </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
@@ -1513,10 +1515,10 @@
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
-        <v>4630</v>
+        <v>109911</v>
       </c>
       <c r="N23" t="n">
-        <v>0.44</v>
+        <v>3.51</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1527,29 +1529,29 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Vermont</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C24" t="n">
-        <v>1377</v>
+        <v>37699</v>
       </c>
       <c r="D24" t="n">
-        <v>56</v>
+        <v>1179</v>
       </c>
       <c r="E24" t="n">
-        <v>159</v>
+        <v>8374</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>391</v>
       </c>
       <c r="G24" t="n">
-        <v>11.9</v>
+        <v>29.24</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>34.79</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
@@ -1558,16 +1560,16 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>1336</v>
+        <v>28639</v>
       </c>
       <c r="L24" t="n">
-        <v>56</v>
+        <v>1124</v>
       </c>
       <c r="M24" t="n">
-        <v>8058</v>
+        <v>704896</v>
       </c>
       <c r="N24" t="n">
-        <v>1.29</v>
+        <v>11.57</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -1578,29 +1580,37 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Connecticut</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44034</v>
-      </c>
-      <c r="C25" t="n">
-        <v>46213</v>
-      </c>
-      <c r="D25" t="n">
-        <v>3530</v>
-      </c>
-      <c r="E25" t="n">
-        <v>6382</v>
-      </c>
-      <c r="F25" t="n">
-        <v>653</v>
+        <v>44035</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>36099</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>267</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>902</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="G25" t="n">
-        <v>13.81</v>
+        <v>2.5</v>
       </c>
       <c r="H25" t="n">
-        <v>18.5</v>
+        <v>1.87</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -1611,10 +1621,10 @@
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
-        <v>378262</v>
+        <v>35862</v>
       </c>
       <c r="N25" t="n">
-        <v>10.56</v>
+        <v>1.18</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -1625,62 +1635,76 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Kansas</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
+          <t>Mississippi</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>44034</v>
+      </c>
+      <c r="C26" t="n">
+        <v>48053</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1436</v>
+      </c>
+      <c r="E26" t="n">
+        <v>21106</v>
+      </c>
+      <c r="F26" t="n">
+        <v>722</v>
+      </c>
+      <c r="G26" t="n">
+        <v>43.92</v>
+      </c>
+      <c r="H26" t="n">
+        <v>50.28</v>
+      </c>
       <c r="I26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="n">
-        <v>169801</v>
+        <v>1125834</v>
       </c>
       <c r="N26" t="n">
-        <v>5.84</v>
+        <v>37.67</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 85', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Texas -- Bexar County</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C27" t="n">
-        <v>42314</v>
+        <v>34633</v>
       </c>
       <c r="D27" t="n">
-        <v>1786</v>
+        <v>298</v>
       </c>
       <c r="E27" t="n">
-        <v>2048</v>
+        <v>464</v>
       </c>
       <c r="F27" t="n">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="G27" t="n">
-        <v>6.16</v>
+        <v>6.81</v>
       </c>
       <c r="H27" t="n">
-        <v>6.9</v>
+        <v>15.32</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
@@ -1689,16 +1713,16 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>33225</v>
+        <v>6812</v>
       </c>
       <c r="L27" t="n">
-        <v>1725</v>
+        <v>111</v>
       </c>
       <c r="M27" t="n">
-        <v>227938</v>
+        <v>146703</v>
       </c>
       <c r="N27" t="n">
-        <v>4.12</v>
+        <v>7.62</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -1709,47 +1733,43 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C28" t="n">
-        <v>23818</v>
+        <v>48721</v>
       </c>
       <c r="D28" t="n">
-        <v>316</v>
+        <v>1561</v>
       </c>
       <c r="E28" t="n">
-        <v>1414</v>
+        <v>9990</v>
       </c>
       <c r="F28" t="n">
-        <v>23</v>
+        <v>150</v>
       </c>
       <c r="G28" t="n">
-        <v>7.69</v>
+        <v>20.5</v>
       </c>
       <c r="H28" t="n">
-        <v>7.72</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="b">
         <v>1</v>
       </c>
-      <c r="K28" t="n">
-        <v>18381</v>
-      </c>
-      <c r="L28" t="n">
-        <v>298</v>
-      </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
       <c r="M28" t="n">
-        <v>90860</v>
+        <v>342186</v>
       </c>
       <c r="N28" t="n">
-        <v>4.77</v>
+        <v>6.19</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -1760,29 +1780,29 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C29" t="n">
-        <v>75868</v>
+        <v>30343</v>
       </c>
       <c r="D29" t="n">
-        <v>6065</v>
+        <v>774</v>
       </c>
       <c r="E29" t="n">
-        <v>21684</v>
+        <v>3644</v>
       </c>
       <c r="F29" t="n">
-        <v>2418</v>
+        <v>96</v>
       </c>
       <c r="G29" t="n">
-        <v>28.58</v>
+        <v>0.12</v>
       </c>
       <c r="H29" t="n">
-        <v>39.87</v>
+        <v>0.12</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -1793,10 +1813,10 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
-        <v>1375424</v>
+        <v>3365783</v>
       </c>
       <c r="N29" t="n">
-        <v>13.81</v>
+        <v>12.07</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -1807,98 +1827,80 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Louisiana</t>
-        </is>
-      </c>
-      <c r="B30" s="2" t="n">
-        <v>44034</v>
-      </c>
-      <c r="C30" t="n">
-        <v>101650</v>
-      </c>
-      <c r="D30" t="n">
-        <v>3574</v>
-      </c>
-      <c r="E30" t="n">
-        <v>36693</v>
-      </c>
-      <c r="F30" t="n">
-        <v>1803</v>
-      </c>
-      <c r="G30" t="n">
-        <v>45.36</v>
-      </c>
-      <c r="H30" t="n">
-        <v>51.05</v>
-      </c>
+          <t>Delaware</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
       <c r="I30" t="b">
         <v>0</v>
       </c>
       <c r="J30" t="b">
-        <v>1</v>
-      </c>
-      <c r="K30" t="n">
-        <v>80885</v>
-      </c>
-      <c r="L30" t="n">
-        <v>3532</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
       <c r="M30" t="n">
-        <v>1502916</v>
+        <v>209892</v>
       </c>
       <c r="N30" t="n">
-        <v>32.23</v>
+        <v>22.11</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... AttributeError("'numpy.float64' object has no attribute 'split'")</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>California</t>
-        </is>
-      </c>
-      <c r="B31" s="3" t="n">
-        <v>44034</v>
+          <t>Nebraska</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>44035</v>
       </c>
       <c r="C31" t="n">
-        <v>425616</v>
+        <v>23818</v>
       </c>
       <c r="D31" t="n">
-        <v>8027</v>
+        <v>316</v>
       </c>
       <c r="E31" t="n">
-        <v>11717</v>
+        <v>1414</v>
       </c>
       <c r="F31" t="n">
-        <v>672</v>
+        <v>23</v>
       </c>
       <c r="G31" t="n">
-        <v>4.31</v>
+        <v>7.69</v>
       </c>
       <c r="H31" t="n">
-        <v>8.6</v>
+        <v>7.72</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
       </c>
       <c r="J31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>271707</v>
+        <v>18381</v>
       </c>
       <c r="L31" t="n">
-        <v>7816</v>
+        <v>298</v>
       </c>
       <c r="M31" t="n">
-        <v>2267875</v>
+        <v>90860</v>
       </c>
       <c r="N31" t="n">
-        <v>5.79</v>
+        <v>4.77</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -1909,43 +1911,47 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Indiana</t>
-        </is>
-      </c>
-      <c r="B32" s="2" t="n">
-        <v>44035</v>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>44034</v>
       </c>
       <c r="C32" t="n">
-        <v>59602</v>
+        <v>425616</v>
       </c>
       <c r="D32" t="n">
-        <v>2683</v>
+        <v>8027</v>
       </c>
       <c r="E32" t="n">
-        <v>6758</v>
+        <v>11717</v>
       </c>
       <c r="F32" t="n">
-        <v>378</v>
+        <v>672</v>
       </c>
       <c r="G32" t="n">
-        <v>11.34</v>
+        <v>4.31</v>
       </c>
       <c r="H32" t="n">
-        <v>14.09</v>
+        <v>8.6</v>
       </c>
       <c r="I32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="b">
-        <v>1</v>
-      </c>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>271707</v>
+      </c>
+      <c r="L32" t="n">
+        <v>7816</v>
+      </c>
       <c r="M32" t="n">
-        <v>619472</v>
+        <v>2267875</v>
       </c>
       <c r="N32" t="n">
-        <v>9.33</v>
+        <v>5.79</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -1956,26 +1962,26 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Alaska</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C33" t="n">
-        <v>2192</v>
+        <v>1377</v>
       </c>
       <c r="D33" t="n">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E33" t="n">
-        <v>52</v>
+        <v>159</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>3.82</v>
+        <v>11.9</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1987,16 +1993,16 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>1361</v>
+        <v>1336</v>
       </c>
       <c r="L33" t="n">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="M33" t="n">
-        <v>24129</v>
+        <v>8058</v>
       </c>
       <c r="N33" t="n">
-        <v>3.27</v>
+        <v>1.29</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2007,47 +2013,39 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C34" t="n">
-        <v>45899</v>
+        <v>18163</v>
       </c>
       <c r="D34" t="n">
-        <v>878</v>
+        <v>596</v>
       </c>
       <c r="E34" t="n">
-        <v>7222</v>
-      </c>
-      <c r="F34" t="n">
-        <v>198</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
-        <v>17.43</v>
-      </c>
-      <c r="H34" t="n">
-        <v>22.97</v>
-      </c>
+        <v>1.81</v>
+      </c>
+      <c r="H34" t="inlineStr"/>
       <c r="I34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="b">
-        <v>1</v>
-      </c>
-      <c r="K34" t="n">
-        <v>41432</v>
-      </c>
-      <c r="L34" t="n">
-        <v>862</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
       <c r="M34" t="n">
-        <v>368744</v>
+        <v>43006</v>
       </c>
       <c r="N34" t="n">
-        <v>6.38</v>
+        <v>2.06</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -2058,43 +2056,43 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C35" t="n">
-        <v>156588</v>
+        <v>385091</v>
       </c>
       <c r="D35" t="n">
-        <v>3360</v>
+        <v>5518</v>
       </c>
       <c r="E35" t="n">
-        <v>40774</v>
+        <v>46054</v>
       </c>
       <c r="F35" t="n">
-        <v>1548</v>
+        <v>1055</v>
       </c>
       <c r="G35" t="n">
-        <v>26.04</v>
+        <v>11.96</v>
       </c>
       <c r="H35" t="n">
-        <v>46.07</v>
+        <v>19.12</v>
       </c>
       <c r="I35" t="b">
         <v>1</v>
       </c>
       <c r="J35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="n">
-        <v>3239300</v>
+        <v>3316376</v>
       </c>
       <c r="N35" t="n">
-        <v>31.46</v>
+        <v>16.1</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -2105,47 +2103,43 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Washington, DC</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C36" t="n">
-        <v>50009</v>
+        <v>11571</v>
       </c>
       <c r="D36" t="n">
-        <v>1482</v>
+        <v>581</v>
       </c>
       <c r="E36" t="n">
-        <v>1766</v>
+        <v>5681</v>
       </c>
       <c r="F36" t="n">
-        <v>49</v>
+        <v>429</v>
       </c>
       <c r="G36" t="n">
-        <v>5.46</v>
+        <v>49.1</v>
       </c>
       <c r="H36" t="n">
-        <v>3.39</v>
+        <v>73.84</v>
       </c>
       <c r="I36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="b">
-        <v>0</v>
-      </c>
-      <c r="K36" t="n">
-        <v>32323</v>
-      </c>
-      <c r="L36" t="n">
-        <v>1446</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
       <c r="M36" t="n">
-        <v>269854</v>
+        <v>321317</v>
       </c>
       <c r="N36" t="n">
-        <v>3.7</v>
+        <v>46.94</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -2156,76 +2150,94 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>New Hampshire</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
+          <t>California - San Francisco</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>44034</v>
+      </c>
+      <c r="C37" t="n">
+        <v>5564</v>
+      </c>
+      <c r="D37" t="n">
+        <v>55</v>
+      </c>
+      <c r="E37" t="n">
+        <v>312</v>
+      </c>
+      <c r="F37" t="n">
+        <v>5</v>
+      </c>
+      <c r="G37" t="n">
+        <v>6.53</v>
+      </c>
+      <c r="H37" t="n">
+        <v>9.619999999999999</v>
+      </c>
       <c r="I37" t="b">
         <v>0</v>
       </c>
       <c r="J37" t="b">
         <v>0</v>
       </c>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="n">
-        <v>20516</v>
-      </c>
-      <c r="N37" t="n">
-        <v>1.53</v>
-      </c>
+      <c r="K37" t="n">
+        <v>4777</v>
+      </c>
+      <c r="L37" t="n">
+        <v>52</v>
+      </c>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 85', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C38" t="n">
-        <v>11571</v>
+        <v>42314</v>
       </c>
       <c r="D38" t="n">
-        <v>581</v>
+        <v>1786</v>
       </c>
       <c r="E38" t="n">
-        <v>5681</v>
+        <v>2048</v>
       </c>
       <c r="F38" t="n">
-        <v>429</v>
+        <v>119</v>
       </c>
       <c r="G38" t="n">
-        <v>49.1</v>
+        <v>6.16</v>
       </c>
       <c r="H38" t="n">
-        <v>73.84</v>
+        <v>6.9</v>
       </c>
       <c r="I38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="b">
-        <v>1</v>
-      </c>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>33225</v>
+      </c>
+      <c r="L38" t="n">
+        <v>1725</v>
+      </c>
       <c r="M38" t="n">
-        <v>321317</v>
+        <v>227938</v>
       </c>
       <c r="N38" t="n">
-        <v>46.94</v>
+        <v>4.12</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -2236,74 +2248,94 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Delaware</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
+          <t>California - San Diego</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>44035</v>
+      </c>
+      <c r="C39" t="n">
+        <v>25608</v>
+      </c>
+      <c r="D39" t="n">
+        <v>512</v>
+      </c>
+      <c r="E39" t="n">
+        <v>942</v>
+      </c>
+      <c r="F39" t="n">
+        <v>19</v>
+      </c>
+      <c r="G39" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H39" t="n">
+        <v>3.81</v>
+      </c>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39" t="b">
         <v>0</v>
       </c>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
+      <c r="K39" t="n">
+        <v>20033</v>
+      </c>
+      <c r="L39" t="n">
+        <v>499</v>
+      </c>
       <c r="M39" t="n">
-        <v>209892</v>
+        <v>166412</v>
       </c>
       <c r="N39" t="n">
-        <v>22.11</v>
+        <v>5.04</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... AttributeError("'numpy.float64' object has no attribute 'split'")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Maine</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C40" t="n">
-        <v>3736</v>
+        <v>16736</v>
       </c>
       <c r="D40" t="n">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="E40" t="n">
-        <v>850</v>
-      </c>
-      <c r="F40" t="inlineStr"/>
+        <v>211</v>
+      </c>
+      <c r="F40" t="n">
+        <v>3</v>
+      </c>
       <c r="G40" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="H40" t="inlineStr"/>
+        <v>1.26</v>
+      </c>
+      <c r="H40" t="n">
+        <v>2.21</v>
+      </c>
       <c r="I40" t="b">
         <v>0</v>
       </c>
       <c r="J40" t="b">
         <v>1</v>
       </c>
-      <c r="K40" t="n">
-        <v>3360</v>
-      </c>
+      <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="n">
-        <v>17881</v>
+        <v>11536</v>
       </c>
       <c r="N40" t="n">
-        <v>1.34</v>
+        <v>0.68</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -2314,109 +2346,145 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Iowa</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
+          <t>Pennsylvania</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>44035</v>
+      </c>
+      <c r="C41" t="n">
+        <v>101408</v>
+      </c>
+      <c r="D41" t="n">
+        <v>7079</v>
+      </c>
+      <c r="E41" t="n">
+        <v>14220</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1484</v>
+      </c>
+      <c r="G41" t="n">
+        <v>30.01</v>
+      </c>
+      <c r="H41" t="n">
+        <v>21.22</v>
+      </c>
       <c r="I41" t="b">
         <v>0</v>
       </c>
       <c r="J41" t="b">
-        <v>0</v>
-      </c>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K41" t="n">
+        <v>47386</v>
+      </c>
+      <c r="L41" t="n">
+        <v>6992</v>
+      </c>
       <c r="M41" t="n">
-        <v>109911</v>
+        <v>1423319</v>
       </c>
       <c r="N41" t="n">
-        <v>3.51</v>
+        <v>11.13</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 85', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>North Carolina</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>44035</v>
+      </c>
+      <c r="C42" t="n">
+        <v>152944</v>
+      </c>
+      <c r="D42" t="n">
+        <v>3063</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3303</v>
+      </c>
+      <c r="F42" t="n">
+        <v>90</v>
+      </c>
+      <c r="G42" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="H42" t="n">
+        <v>3.53</v>
+      </c>
       <c r="I42" t="b">
         <v>0</v>
       </c>
       <c r="J42" t="b">
         <v>0</v>
       </c>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
+      <c r="K42" t="n">
+        <v>76501</v>
+      </c>
+      <c r="L42" t="n">
+        <v>2552</v>
+      </c>
       <c r="M42" t="n">
-        <v>2179622</v>
+        <v>305259</v>
       </c>
       <c r="N42" t="n">
-        <v>21.46</v>
+        <v>4.39</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 85', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C43" t="n">
-        <v>166925</v>
+        <v>156588</v>
       </c>
       <c r="D43" t="n">
-        <v>7367</v>
+        <v>3360</v>
       </c>
       <c r="E43" t="n">
-        <v>27933</v>
+        <v>40774</v>
       </c>
       <c r="F43" t="n">
-        <v>2027</v>
+        <v>1548</v>
       </c>
       <c r="G43" t="n">
-        <v>16.73</v>
+        <v>26.04</v>
       </c>
       <c r="H43" t="n">
-        <v>27.51</v>
+        <v>46.07</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
       </c>
       <c r="J43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="n">
-        <v>1824125</v>
+        <v>3239300</v>
       </c>
       <c r="N43" t="n">
-        <v>14.23</v>
+        <v>31.46</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -2427,62 +2495,76 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Idaho</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>44033</v>
+      </c>
+      <c r="C44" t="n">
+        <v>79371</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2048</v>
+      </c>
+      <c r="E44" t="n">
+        <v>12922</v>
+      </c>
+      <c r="F44" t="n">
+        <v>483</v>
+      </c>
+      <c r="G44" t="n">
+        <v>16.28</v>
+      </c>
+      <c r="H44" t="n">
+        <v>23.58</v>
+      </c>
       <c r="I44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="n">
-        <v>11536</v>
+        <v>1613285</v>
       </c>
       <c r="N44" t="n">
-        <v>0.68</v>
+        <v>19.17</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 85', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
         <v>44035</v>
       </c>
       <c r="C45" t="n">
-        <v>48721</v>
+        <v>59602</v>
       </c>
       <c r="D45" t="n">
-        <v>1561</v>
+        <v>2683</v>
       </c>
       <c r="E45" t="n">
-        <v>9990</v>
+        <v>6758</v>
       </c>
       <c r="F45" t="n">
-        <v>150</v>
+        <v>378</v>
       </c>
       <c r="G45" t="n">
-        <v>20.5</v>
+        <v>11.34</v>
       </c>
       <c r="H45" t="n">
-        <v>9.609999999999999</v>
+        <v>14.09</v>
       </c>
       <c r="I45" t="b">
         <v>1</v>
@@ -2493,10 +2575,10 @@
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="n">
-        <v>342186</v>
+        <v>619472</v>
       </c>
       <c r="N45" t="n">
-        <v>6.19</v>
+        <v>9.33</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -2507,43 +2589,47 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>New Hampshire</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>44034</v>
+        <v>44035</v>
       </c>
       <c r="C46" t="n">
-        <v>114320</v>
+        <v>6318</v>
       </c>
       <c r="D46" t="n">
-        <v>8468</v>
+        <v>405</v>
       </c>
       <c r="E46" t="n">
-        <v>10731</v>
+        <v>327</v>
       </c>
       <c r="F46" t="n">
-        <v>693</v>
+        <v>9</v>
       </c>
       <c r="G46" t="n">
-        <v>9.390000000000001</v>
+        <v>6.03</v>
       </c>
       <c r="H46" t="n">
-        <v>8.18</v>
+        <v>2.23</v>
       </c>
       <c r="I46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" t="b">
         <v>0</v>
       </c>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
+      <c r="K46" t="n">
+        <v>5426</v>
+      </c>
+      <c r="L46" t="n">
+        <v>403</v>
+      </c>
       <c r="M46" t="n">
-        <v>510558</v>
+        <v>20516</v>
       </c>
       <c r="N46" t="n">
-        <v>7.48</v>
+        <v>1.53</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -2554,98 +2640,80 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Wisconsin -- Milwaukee</t>
-        </is>
-      </c>
-      <c r="B47" s="2" t="n">
-        <v>44035</v>
-      </c>
-      <c r="C47" t="n">
-        <v>17162</v>
-      </c>
-      <c r="D47" t="n">
-        <v>374</v>
-      </c>
-      <c r="E47" t="n">
-        <v>4842</v>
-      </c>
-      <c r="F47" t="n">
-        <v>147</v>
-      </c>
-      <c r="G47" t="n">
-        <v>30.44</v>
-      </c>
-      <c r="H47" t="n">
-        <v>39.3</v>
-      </c>
+          <t>Kentucky</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
       <c r="I47" t="b">
         <v>0</v>
       </c>
       <c r="J47" t="b">
         <v>0</v>
       </c>
-      <c r="K47" t="n">
-        <v>15909</v>
-      </c>
-      <c r="L47" t="n">
-        <v>374</v>
-      </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
       <c r="M47" t="n">
-        <v>252321</v>
+        <v>354112</v>
       </c>
       <c r="N47" t="n">
-        <v>26.44</v>
+        <v>7.98</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... UnboundLocalError("local variable 'aa_deaths_pct' referenced before assignment")</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>California - Los Angeles</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>44035</v>
+        <v>44034</v>
       </c>
       <c r="C48" t="n">
-        <v>37699</v>
+        <v>166848</v>
       </c>
       <c r="D48" t="n">
-        <v>1179</v>
+        <v>4262</v>
       </c>
       <c r="E48" t="n">
-        <v>8374</v>
+        <v>4451</v>
       </c>
       <c r="F48" t="n">
-        <v>391</v>
+        <v>424</v>
       </c>
       <c r="G48" t="n">
-        <v>29.24</v>
+        <v>4.64</v>
       </c>
       <c r="H48" t="n">
-        <v>34.79</v>
+        <v>10.66</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
       </c>
       <c r="J48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48" t="n">
-        <v>28639</v>
+        <v>95952</v>
       </c>
       <c r="L48" t="n">
-        <v>1124</v>
+        <v>3976</v>
       </c>
       <c r="M48" t="n">
-        <v>704896</v>
+        <v>823987</v>
       </c>
       <c r="N48" t="n">
-        <v>11.57</v>
+        <v>8.16</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>

</xml_diff>